<commit_message>
Changes in benchmarks and minor changes in sections 2 and 3
</commit_message>
<xml_diff>
--- a/Benchmark.xlsx
+++ b/Benchmark.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Iteration 1</t>
   </si>
@@ -55,76 +54,10 @@
     <t>100 nodes</t>
   </si>
   <si>
-    <t>200 nodes</t>
-  </si>
-  <si>
-    <t>300 nodes</t>
-  </si>
-  <si>
-    <t>400 nodes</t>
-  </si>
-  <si>
     <t>500 nodes</t>
   </si>
   <si>
-    <t>600 nodes</t>
-  </si>
-  <si>
-    <t>700 nodes</t>
-  </si>
-  <si>
-    <t>800 nodes</t>
-  </si>
-  <si>
-    <t>900 nodes</t>
-  </si>
-  <si>
     <t>1000 nodes</t>
-  </si>
-  <si>
-    <t>1600 nodes</t>
-  </si>
-  <si>
-    <t>3200 nodes</t>
-  </si>
-  <si>
-    <t>6400 nodes</t>
-  </si>
-  <si>
-    <t>10 edges</t>
-  </si>
-  <si>
-    <t>20 edges</t>
-  </si>
-  <si>
-    <t>30 edges</t>
-  </si>
-  <si>
-    <t>40 edges</t>
-  </si>
-  <si>
-    <t>50 edges</t>
-  </si>
-  <si>
-    <t>60 edges</t>
-  </si>
-  <si>
-    <t>70 edges</t>
-  </si>
-  <si>
-    <t>80 edges</t>
-  </si>
-  <si>
-    <t>90 edges</t>
-  </si>
-  <si>
-    <t>100 edges</t>
-  </si>
-  <si>
-    <t>200 edges</t>
-  </si>
-  <si>
-    <t>300 edges</t>
   </si>
   <si>
     <t>5 nodes</t>
@@ -307,28 +240,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-AR"/>
-              <a:t>Many nodes</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13538486677492162"/>
+          <c:y val="4.8615294016645501E-2"/>
+          <c:w val="0.58357772399072683"/>
+          <c:h val="0.71380754753801501"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -337,62 +261,57 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Without cache</c:v>
+            <c:v>Before refactoring</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$B$3:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
+            <c:numRef>
+              <c:f>Hoja1!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>100 nodes</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200 nodes</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300 nodes</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400 nodes</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500 nodes</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600 nodes</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700 nodes</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800 nodes</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900 nodes</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000 nodes</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1600 nodes</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3200 nodes</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6400 nodes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$M$3:$M$15</c:f>
+              <c:f>Hoja1!$M$3:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>13.6</c:v>
                 </c:pt>
@@ -425,12 +344,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>110.7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>256.10000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>382.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,62 +353,57 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>With cache</c:v>
+            <c:v>After refactoring</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$B$3:$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
+            <c:numRef>
+              <c:f>Hoja1!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>100 nodes</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200 nodes</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300 nodes</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400 nodes</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500 nodes</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600 nodes</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700 nodes</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800 nodes</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900 nodes</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000 nodes</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1600 nodes</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3200 nodes</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6400 nodes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$Y$3:$Y$15</c:f>
+              <c:f>Hoja1!$Y$3:$Y$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>13.9</c:v>
                 </c:pt>
@@ -528,12 +436,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>102.7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>209.9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>410.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -548,20 +450,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="96365056"/>
-        <c:axId val="68141632"/>
+        <c:axId val="56323072"/>
+        <c:axId val="90309184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96365056"/>
+        <c:axId val="56323072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68141632"/>
+        <c:crossAx val="90309184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -569,35 +491,68 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68141632"/>
+        <c:axId val="90309184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Time in ms.</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96365056"/>
+        <c:crossAx val="56323072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.63732855377513598"/>
+          <c:y val="0.82831976549142294"/>
+          <c:w val="0.25372200349956253"/>
+          <c:h val="0.16743438320209975"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -616,28 +571,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-AR"/>
-              <a:t>Many edges</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10929744892999486"/>
+          <c:y val="4.8456177164267894E-2"/>
+          <c:w val="0.77782777152855909"/>
+          <c:h val="0.71474424951896753"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -645,60 +591,52 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Without cache</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$B$16:$B$27</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
+            <c:numRef>
+              <c:f>Hoja1!$B$16:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10 edges</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20 edges</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30 edges</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40 edges</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50 edges</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60 edges</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70 edges</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80 edges</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90 edges</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100 edges</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>200 edges</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300 edges</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$M$16:$M$27</c:f>
+              <c:f>Hoja1!$M$16:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.6</c:v>
                 </c:pt>
@@ -712,7 +650,7 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>121.8</c:v>
+                  <c:v>43.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>63.9</c:v>
@@ -727,13 +665,7 @@
                   <c:v>143.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>269.89999999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1132.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4122.3999999999996</c:v>
+                  <c:v>167.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -742,60 +674,52 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>With cache</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$B$16:$B$27</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
+            <c:numRef>
+              <c:f>Hoja1!$B$16:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10 edges</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20 edges</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30 edges</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40 edges</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50 edges</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60 edges</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70 edges</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80 edges</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90 edges</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100 edges</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>200 edges</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>300 edges</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$Y$16:$Y$27</c:f>
+              <c:f>Hoja1!$Y$16:$Y$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.5</c:v>
                 </c:pt>
@@ -815,7 +739,7 @@
                   <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150</c:v>
+                  <c:v>86.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>109.5</c:v>
@@ -824,13 +748,7 @@
                   <c:v>149.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>192.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1195.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3645.4</c:v>
+                  <c:v>181.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,20 +763,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41218048"/>
-        <c:axId val="68143360"/>
+        <c:axId val="90130432"/>
+        <c:axId val="90310912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41218048"/>
+        <c:axId val="90130432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Edges</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68143360"/>
+        <c:crossAx val="90310912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,7 +804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68143360"/>
+        <c:axId val="90310912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -877,20 +815,21 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41218048"/>
+        <c:crossAx val="90130432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1070,11 +1009,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41218560"/>
-        <c:axId val="68145088"/>
+        <c:axId val="90130944"/>
+        <c:axId val="90312640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41218560"/>
+        <c:axId val="90130944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1083,7 +1022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68145088"/>
+        <c:crossAx val="90312640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1091,7 +1030,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68145088"/>
+        <c:axId val="90312640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41218560"/>
+        <c:crossAx val="90130944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1196,6 +1135,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1312,6 +1252,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1331,15 +1272,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1360,16 +1301,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1770,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1736,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1840,7 +1781,7 @@
         <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
         <v>0</v>
@@ -1873,18 +1814,18 @@
         <v>10</v>
       </c>
       <c r="Y2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="Z2" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -1960,8 +1901,8 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4">
+        <v>200</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -2037,8 +1978,8 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>13</v>
+      <c r="B5">
+        <v>300</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -2114,8 +2055,8 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>14</v>
+      <c r="B6">
+        <v>400</v>
       </c>
       <c r="C6">
         <v>23</v>
@@ -2191,8 +2132,8 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="B7">
+        <v>500</v>
       </c>
       <c r="C7">
         <v>31</v>
@@ -2268,8 +2209,8 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>16</v>
+      <c r="B8">
+        <v>600</v>
       </c>
       <c r="C8">
         <v>36</v>
@@ -2345,8 +2286,8 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>17</v>
+      <c r="B9">
+        <v>700</v>
       </c>
       <c r="C9">
         <v>41</v>
@@ -2422,8 +2363,8 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>18</v>
+      <c r="B10">
+        <v>800</v>
       </c>
       <c r="C10">
         <v>47</v>
@@ -2499,8 +2440,8 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>19</v>
+      <c r="B11">
+        <v>900</v>
       </c>
       <c r="C11">
         <v>54</v>
@@ -2576,8 +2517,8 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>20</v>
+      <c r="B12">
+        <v>1000</v>
       </c>
       <c r="C12">
         <v>58</v>
@@ -2653,8 +2594,8 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>21</v>
+      <c r="B13">
+        <v>1600</v>
       </c>
       <c r="C13">
         <v>255</v>
@@ -2730,8 +2671,8 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>22</v>
+      <c r="B14">
+        <v>3200</v>
       </c>
       <c r="C14">
         <v>180</v>
@@ -2807,8 +2748,8 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>23</v>
+      <c r="B15">
+        <v>6400</v>
       </c>
       <c r="C15">
         <v>358</v>
@@ -2885,10 +2826,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2964,8 +2905,8 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>25</v>
+      <c r="B17">
+        <v>20</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -3041,8 +2982,8 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>26</v>
+      <c r="B18">
+        <v>30</v>
       </c>
       <c r="C18">
         <v>16</v>
@@ -3118,8 +3059,8 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>27</v>
+      <c r="B19">
+        <v>40</v>
       </c>
       <c r="C19">
         <v>111</v>
@@ -3195,42 +3136,42 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>28</v>
+      <c r="B20">
+        <v>50</v>
       </c>
       <c r="C20">
         <v>41</v>
       </c>
       <c r="D20">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="E20">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="F20">
-        <v>129</v>
+        <v>45</v>
       </c>
       <c r="G20">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="H20">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="I20">
-        <v>137</v>
+        <v>44</v>
       </c>
       <c r="J20">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="K20">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="L20">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="M20">
         <f t="shared" si="0"/>
-        <v>121.8</v>
+        <v>43.7</v>
       </c>
       <c r="O20">
         <v>42</v>
@@ -3268,12 +3209,12 @@
       </c>
       <c r="Z20">
         <f t="shared" si="2"/>
-        <v>-64.039408866995075</v>
+        <v>0.2288329519450798</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>29</v>
+      <c r="B21">
+        <v>60</v>
       </c>
       <c r="C21">
         <v>60</v>
@@ -3349,8 +3290,8 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>30</v>
+      <c r="B22">
+        <v>70</v>
       </c>
       <c r="C22">
         <v>81</v>
@@ -3390,13 +3331,13 @@
         <v>79</v>
       </c>
       <c r="P22">
-        <v>172</v>
+        <v>87</v>
       </c>
       <c r="Q22">
-        <v>184</v>
+        <v>91</v>
       </c>
       <c r="R22">
-        <v>175</v>
+        <v>82</v>
       </c>
       <c r="S22">
         <v>91</v>
@@ -3405,29 +3346,29 @@
         <v>83</v>
       </c>
       <c r="U22">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="V22">
-        <v>178</v>
+        <v>88</v>
       </c>
       <c r="W22">
-        <v>179</v>
+        <v>85</v>
       </c>
       <c r="X22">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="Y22">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>86.9</v>
       </c>
       <c r="Z22">
         <f t="shared" si="2"/>
-        <v>80.072028811524603</v>
+        <v>4.3217286914765936</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>31</v>
+      <c r="B23">
+        <v>80</v>
       </c>
       <c r="C23">
         <v>104</v>
@@ -3503,8 +3444,8 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>32</v>
+      <c r="B24">
+        <v>90</v>
       </c>
       <c r="C24">
         <v>138</v>
@@ -3580,45 +3521,45 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>33</v>
+      <c r="B25">
+        <v>100</v>
       </c>
       <c r="C25">
-        <v>270</v>
+        <v>163</v>
       </c>
       <c r="D25">
-        <v>256</v>
+        <v>165</v>
       </c>
       <c r="E25">
-        <v>265</v>
+        <v>164</v>
       </c>
       <c r="F25">
-        <v>317</v>
+        <v>171</v>
       </c>
       <c r="G25">
-        <v>272</v>
+        <v>165</v>
       </c>
       <c r="H25">
-        <v>266</v>
+        <v>167</v>
       </c>
       <c r="I25">
-        <v>261</v>
+        <v>172</v>
       </c>
       <c r="J25">
-        <v>266</v>
+        <v>164</v>
       </c>
       <c r="K25">
-        <v>266</v>
+        <v>171</v>
       </c>
       <c r="L25">
-        <v>260</v>
+        <v>169</v>
       </c>
       <c r="M25">
         <f t="shared" si="0"/>
-        <v>269.89999999999998</v>
+        <v>167.1</v>
       </c>
       <c r="O25">
-        <v>276</v>
+        <v>170</v>
       </c>
       <c r="P25">
         <v>169</v>
@@ -3649,16 +3590,16 @@
       </c>
       <c r="Y25">
         <f t="shared" si="1"/>
-        <v>192.3</v>
+        <v>181.7</v>
       </c>
       <c r="Z25">
         <f t="shared" si="2"/>
-        <v>-28.751389403482762</v>
+        <v>8.7372830640335195</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>34</v>
+      <c r="B26">
+        <v>200</v>
       </c>
       <c r="C26">
         <v>1024</v>
@@ -3734,8 +3675,8 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>35</v>
+      <c r="B27">
+        <v>300</v>
       </c>
       <c r="C27">
         <v>3585</v>
@@ -3812,10 +3753,10 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>152</v>
@@ -3892,7 +3833,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C29">
         <v>2498</v>
@@ -3969,7 +3910,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C30">
         <v>10910</v>
@@ -4046,10 +3987,10 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>312</v>
@@ -4126,7 +4067,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C32">
         <v>951</v>
@@ -4203,7 +4144,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C33">
         <v>10165</v>
@@ -4280,10 +4221,10 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>11</v>
@@ -4360,7 +4301,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>269</v>
@@ -4437,7 +4378,7 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C36">
         <v>3772</v>
@@ -4514,7 +4455,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C37">
         <v>39937</v>
@@ -4591,7 +4532,7 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -4671,7 +4612,7 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>8</v>
@@ -4748,7 +4689,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C40">
         <v>12</v>
@@ -4825,7 +4766,7 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C41">
         <v>14</v>
@@ -4902,7 +4843,7 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C42">
         <v>17</v>
@@ -4979,7 +4920,7 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C43">
         <v>20</v>
@@ -5056,10 +4997,10 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C44">
         <v>3959</v>
@@ -5136,10 +5077,10 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C45">
         <v>173</v>
@@ -5216,10 +5157,10 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C46">
         <v>5053</v>
@@ -5296,64 +5237,64 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="T48" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="W48" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="X48" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="19:25" x14ac:dyDescent="0.25">
       <c r="S49" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="T49">
         <v>18</v>
       </c>
       <c r="W49" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="X49">
         <v>4</v>
       </c>
       <c r="Y49" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="19:25" x14ac:dyDescent="0.25">
       <c r="S50" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="T50">
         <v>24</v>
       </c>
       <c r="W50" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="X50">
         <v>1</v>
       </c>
       <c r="Y50" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="19:25" x14ac:dyDescent="0.25">
       <c r="S51" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="T51">
         <v>2</v>
       </c>
       <c r="W51" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="X51">
         <v>2</v>
       </c>
       <c r="Y51" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="19:25" x14ac:dyDescent="0.25">
@@ -5361,57 +5302,57 @@
         <v>44</v>
       </c>
       <c r="W52" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="X52">
         <v>11</v>
       </c>
       <c r="Y52" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="19:25" x14ac:dyDescent="0.25">
       <c r="W53" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="X53">
         <v>10</v>
       </c>
       <c r="Y53" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="19:25" x14ac:dyDescent="0.25">
       <c r="W54" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="X54">
         <v>11</v>
       </c>
       <c r="Y54" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="19:25" x14ac:dyDescent="0.25">
       <c r="W55" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="X55">
         <v>1</v>
       </c>
       <c r="Y55" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="19:25" x14ac:dyDescent="0.25">
       <c r="W56" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="X56">
         <v>4</v>
       </c>
       <c r="Y56" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -5420,7 +5361,7 @@
     <mergeCell ref="O1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>